<commit_message>
Add more Cal. points
</commit_message>
<xml_diff>
--- a/Methods/dataBase.xlsx
+++ b/Methods/dataBase.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2304" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3184" uniqueCount="194">
   <si>
     <t xml:space="preserve">Real_X</t>
   </si>
@@ -228,6 +228,24 @@
   </si>
   <si>
     <t xml:space="preserve">-34.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-71.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-73.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-33.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-70.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-32.00</t>
   </si>
   <si>
     <t xml:space="preserve">-48.8</t>
@@ -685,10 +703,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H261"/>
+  <dimension ref="A1:H371"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A235" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A252" activeCellId="0" sqref="A252"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A349" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B371" activeCellId="0" sqref="A363:B371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7487,6 +7505,2866 @@
       </c>
       <c r="H261" s="0" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B262" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C262" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D262" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E262" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F262" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G262" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="H262" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B263" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C263" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D263" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E263" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F263" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G263" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H263" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B264" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C264" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D264" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E264" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F264" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G264" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H264" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B265" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C265" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D265" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E265" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F265" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G265" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H265" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B266" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C266" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D266" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E266" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F266" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G266" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H266" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B267" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C267" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D267" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E267" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F267" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G267" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H267" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B268" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C268" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D268" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E268" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F268" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G268" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H268" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B269" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C269" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D269" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E269" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F269" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G269" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H269" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B270" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C270" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D270" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E270" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F270" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G270" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="H270" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B271" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C271" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D271" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E271" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F271" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G271" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="H271" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B272" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C272" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D272" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E272" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F272" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G272" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H272" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B273" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C273" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D273" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E273" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F273" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G273" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H273" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B274" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C274" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D274" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E274" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F274" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G274" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H274" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B275" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C275" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D275" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E275" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F275" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G275" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H275" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B276" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C276" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D276" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E276" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F276" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G276" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H276" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B277" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C277" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D277" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E277" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F277" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G277" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H277" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B278" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C278" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D278" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E278" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F278" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G278" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H278" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B279" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C279" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D279" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E279" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F279" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G279" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H279" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B280" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C280" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D280" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E280" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F280" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G280" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H280" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B281" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C281" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D281" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E281" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F281" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G281" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H281" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B282" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C282" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D282" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E282" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F282" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G282" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H282" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B283" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C283" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D283" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E283" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F283" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G283" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H283" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B284" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C284" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D284" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E284" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F284" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G284" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H284" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B285" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C285" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D285" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E285" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F285" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G285" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H285" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B286" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C286" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D286" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E286" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F286" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G286" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H286" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B287" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C287" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D287" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E287" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F287" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G287" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H287" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B288" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C288" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D288" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E288" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F288" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G288" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H288" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B289" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C289" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D289" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E289" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F289" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G289" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H289" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B290" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C290" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D290" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E290" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F290" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G290" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H290" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B291" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C291" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D291" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E291" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F291" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G291" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H291" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B292" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C292" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D292" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E292" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F292" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="G292" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H292" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B293" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C293" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D293" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E293" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F293" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G293" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H293" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B294" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C294" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D294" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E294" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F294" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G294" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H294" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B295" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C295" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D295" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E295" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F295" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G295" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H295" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B296" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C296" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D296" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E296" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F296" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G296" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H296" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B297" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C297" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D297" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E297" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F297" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G297" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H297" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B298" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C298" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D298" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E298" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F298" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G298" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H298" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B299" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C299" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D299" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E299" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F299" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G299" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H299" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B300" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C300" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D300" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E300" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F300" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G300" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H300" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B301" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C301" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D301" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E301" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F301" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G301" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H301" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B302" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C302" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D302" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E302" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F302" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G302" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H302" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B303" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C303" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D303" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E303" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F303" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G303" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H303" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B304" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C304" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D304" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E304" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F304" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G304" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H304" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B305" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C305" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D305" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E305" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F305" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G305" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H305" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B306" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C306" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D306" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E306" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F306" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G306" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H306" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B307" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C307" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D307" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E307" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F307" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G307" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H307" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B308" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C308" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D308" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E308" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F308" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G308" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H308" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B309" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C309" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D309" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E309" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F309" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G309" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H309" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B310" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C310" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D310" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E310" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F310" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G310" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H310" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B311" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C311" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D311" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E311" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F311" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G311" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H311" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B312" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C312" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D312" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E312" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F312" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G312" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H312" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B313" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C313" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D313" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E313" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F313" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G313" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H313" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B314" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C314" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D314" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E314" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F314" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G314" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H314" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B315" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C315" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D315" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E315" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F315" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G315" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H315" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B316" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C316" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D316" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E316" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F316" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G316" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H316" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B317" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C317" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D317" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E317" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F317" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G317" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H317" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B318" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C318" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D318" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E318" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F318" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G318" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H318" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B319" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C319" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D319" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E319" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F319" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G319" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H319" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B320" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C320" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D320" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E320" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F320" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G320" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H320" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B321" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C321" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D321" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E321" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F321" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G321" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H321" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B322" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C322" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D322" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E322" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F322" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G322" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H322" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B323" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C323" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D323" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E323" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F323" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G323" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H323" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B324" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C324" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D324" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E324" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F324" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G324" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H324" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B325" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C325" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D325" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E325" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F325" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G325" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H325" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B326" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C326" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D326" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E326" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F326" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G326" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H326" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B327" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C327" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D327" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E327" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F327" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G327" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H327" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B328" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C328" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D328" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E328" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F328" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G328" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H328" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B329" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C329" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D329" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E329" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F329" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G329" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H329" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B330" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C330" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D330" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E330" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F330" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G330" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H330" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B331" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C331" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D331" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E331" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F331" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G331" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H331" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B332" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C332" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D332" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E332" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F332" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G332" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H332" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B333" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C333" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D333" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E333" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F333" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G333" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H333" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B334" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C334" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D334" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E334" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F334" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G334" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H334" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B335" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C335" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D335" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E335" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F335" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G335" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H335" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B336" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C336" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D336" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E336" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F336" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G336" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H336" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B337" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C337" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D337" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E337" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F337" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G337" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H337" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B338" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C338" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D338" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E338" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F338" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G338" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H338" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B339" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C339" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D339" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E339" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F339" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G339" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H339" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B340" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C340" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D340" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E340" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F340" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G340" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H340" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B341" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C341" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D341" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E341" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F341" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G341" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H341" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B342" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C342" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D342" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E342" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F342" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G342" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H342" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B343" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C343" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D343" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E343" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F343" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="G343" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H343" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B344" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C344" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D344" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E344" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F344" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G344" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H344" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B345" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C345" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D345" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E345" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F345" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G345" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H345" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B346" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C346" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D346" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E346" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F346" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G346" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H346" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B347" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C347" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D347" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E347" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F347" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G347" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H347" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B348" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C348" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D348" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E348" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F348" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G348" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H348" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B349" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C349" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D349" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E349" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F349" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G349" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H349" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B350" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C350" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D350" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E350" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F350" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G350" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H350" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B351" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C351" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D351" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E351" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F351" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G351" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H351" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B352" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C352" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D352" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E352" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F352" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G352" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H352" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A353" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B353" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C353" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D353" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E353" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F353" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G353" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H353" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A354" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B354" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C354" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D354" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E354" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F354" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G354" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H354" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B355" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C355" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D355" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E355" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F355" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G355" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H355" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B356" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C356" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D356" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E356" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F356" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G356" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H356" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B357" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C357" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D357" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E357" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F357" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G357" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H357" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B358" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C358" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D358" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E358" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F358" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G358" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H358" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B359" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C359" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D359" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E359" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F359" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G359" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H359" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B360" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C360" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D360" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E360" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F360" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G360" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H360" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A361" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B361" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C361" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D361" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E361" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F361" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G361" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H361" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B362" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C362" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D362" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E362" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F362" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G362" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H362" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B363" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C363" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D363" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E363" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F363" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G363" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H363" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B364" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C364" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D364" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E364" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F364" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G364" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H364" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B365" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C365" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D365" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E365" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F365" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G365" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H365" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A366" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B366" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C366" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D366" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E366" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F366" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G366" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H366" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B367" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C367" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D367" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E367" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F367" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G367" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H367" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A368" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B368" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C368" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D368" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E368" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F368" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G368" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H368" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A369" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B369" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C369" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D369" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E369" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F369" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G369" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H369" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A370" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B370" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C370" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D370" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E370" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F370" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G370" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H370" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A371" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B371" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C371" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D371" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E371" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F371" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G371" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H371" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -7507,8 +10385,8 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I20" activeCellId="1" sqref="A363:B371 I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7518,7 +10396,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -7556,22 +10434,22 @@
         <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7582,22 +10460,22 @@
         <v>24</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7608,22 +10486,22 @@
         <v>40</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7634,22 +10512,22 @@
         <v>45</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>83</v>
-      </c>
       <c r="H5" s="0" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7660,22 +10538,22 @@
         <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7686,22 +10564,22 @@
         <v>56</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7712,22 +10590,22 @@
         <v>24</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7738,22 +10616,22 @@
         <v>45</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7764,22 +10642,22 @@
         <v>9</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7790,22 +10668,22 @@
         <v>56</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7816,22 +10694,22 @@
         <v>24</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7842,22 +10720,22 @@
         <v>45</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7868,22 +10746,22 @@
         <v>9</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7894,22 +10772,22 @@
         <v>56</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7920,22 +10798,22 @@
         <v>63</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7946,22 +10824,22 @@
         <v>24</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7972,22 +10850,22 @@
         <v>40</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7998,22 +10876,22 @@
         <v>45</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8024,22 +10902,22 @@
         <v>9</v>
       </c>
       <c r="C20" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G20" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>156</v>
-      </c>
       <c r="H20" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8050,22 +10928,22 @@
         <v>65</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8076,22 +10954,22 @@
         <v>56</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8102,22 +10980,22 @@
         <v>63</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8128,22 +11006,22 @@
         <v>24</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8154,22 +11032,22 @@
         <v>66</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8180,22 +11058,22 @@
         <v>40</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8206,22 +11084,22 @@
         <v>67</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>